<commit_message>
Various changes to class tables, core rules, and exploits
</commit_message>
<xml_diff>
--- a/Development/Spreadsheets/CBE+Weapon Master+Signature Weapon Ranger DPR (no crits).xlsx
+++ b/Development/Spreadsheets/CBE+Weapon Master+Signature Weapon Ranger DPR (no crits).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Aetherwynn-Unstable-Isotopes\Development\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D6C059-DED1-4AC2-9BEF-D315E6E757F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E05A65-0673-4567-8DFA-7BD310646C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C602150E-3BDC-4B64-9334-AA1DC424628B}"/>
   </bookViews>
@@ -437,7 +437,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$1</c15:sqref>
@@ -466,7 +466,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$2:$B$21</c15:sqref>
@@ -540,7 +540,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-CB17-4BB3-8030-97FF44B26EAC}"/>
                   </c:ext>
@@ -553,7 +553,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$1</c15:sqref>
@@ -582,7 +582,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$C$2:$C$21</c15:sqref>
@@ -656,7 +656,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-CB17-4BB3-8030-97FF44B26EAC}"/>
                   </c:ext>
@@ -669,7 +669,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$1</c15:sqref>
@@ -698,7 +698,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$2:$D$21</c15:sqref>
@@ -772,7 +772,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-CB17-4BB3-8030-97FF44B26EAC}"/>
                   </c:ext>
@@ -785,7 +785,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$E$1</c15:sqref>
@@ -814,7 +814,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$E$2:$E$21</c15:sqref>
@@ -888,7 +888,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-CB17-4BB3-8030-97FF44B26EAC}"/>
                   </c:ext>
@@ -901,7 +901,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$F$1</c15:sqref>
@@ -930,7 +930,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$F$2:$F$21</c15:sqref>
@@ -1004,7 +1004,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-CB17-4BB3-8030-97FF44B26EAC}"/>
                   </c:ext>
@@ -1017,7 +1017,7 @@
                 <c:order val="6"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$G$1</c15:sqref>
@@ -1048,7 +1048,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$G$2:$G$21</c15:sqref>
@@ -1122,7 +1122,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-CB17-4BB3-8030-97FF44B26EAC}"/>
                   </c:ext>
@@ -1135,7 +1135,7 @@
                 <c:order val="7"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$H$1</c15:sqref>
@@ -1166,7 +1166,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$H$2:$H$21</c15:sqref>
@@ -1240,7 +1240,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-CB17-4BB3-8030-97FF44B26EAC}"/>
                   </c:ext>
@@ -1253,7 +1253,7 @@
                 <c:order val="8"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$1</c15:sqref>
@@ -1284,7 +1284,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$2:$I$21</c15:sqref>
@@ -1358,7 +1358,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-CB17-4BB3-8030-97FF44B26EAC}"/>
                   </c:ext>
@@ -1371,7 +1371,7 @@
                 <c:order val="9"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$J$1</c15:sqref>
@@ -1402,7 +1402,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$J$2:$J$21</c15:sqref>
@@ -1476,7 +1476,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-CB17-4BB3-8030-97FF44B26EAC}"/>
                   </c:ext>
@@ -1489,7 +1489,7 @@
                 <c:order val="10"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$K$1</c15:sqref>
@@ -1520,7 +1520,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$K$2:$K$21</c15:sqref>
@@ -1594,7 +1594,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000A-CB17-4BB3-8030-97FF44B26EAC}"/>
                   </c:ext>
@@ -1607,7 +1607,7 @@
                 <c:order val="11"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$L$1</c15:sqref>
@@ -1638,7 +1638,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$L$2:$L$21</c15:sqref>
@@ -1712,7 +1712,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000B-CB17-4BB3-8030-97FF44B26EAC}"/>
                   </c:ext>
@@ -1725,7 +1725,7 @@
                 <c:order val="12"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$M$1</c15:sqref>
@@ -1757,7 +1757,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$M$2:$M$21</c15:sqref>
@@ -1831,7 +1831,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000C-CB17-4BB3-8030-97FF44B26EAC}"/>
                   </c:ext>
@@ -1988,6 +1988,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1995,7 +1996,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2961,7 +2961,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3093,7 +3093,7 @@
         <v>5</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L21" si="1">(21 - (J3 - K3)) / 20</f>
+        <f>(21 - (J3 - K3)) / 20</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="M3">
@@ -3140,14 +3140,14 @@
         <v>5</v>
       </c>
       <c r="L4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="L3:L21" si="1">(21 - (J4 - K4)) / 20</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="M4">
         <v>3.5</v>
       </c>
       <c r="N4" s="2">
-        <f t="shared" ref="N3:N21" si="2">(G4+F4)*L4*(M4+D4+E4+I4+C4)</f>
+        <f t="shared" ref="N4:N21" si="2">(G4+F4)*L4*(M4+D4+E4+I4+C4)</f>
         <v>13.200000000000001</v>
       </c>
     </row>
@@ -3375,14 +3375,14 @@
         <v>10</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" si="1"/>
+        <f>(21 - (J9 - K9)) / 20</f>
         <v>0.8</v>
       </c>
       <c r="M9">
         <v>3.5</v>
       </c>
       <c r="N9" s="2">
-        <f t="shared" si="2"/>
+        <f>(G9+F9)*L9*(M9+D9+E9+I9+C9)</f>
         <v>36.000000000000007</v>
       </c>
     </row>
@@ -3563,14 +3563,14 @@
         <v>11</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" si="1"/>
+        <f>(21 - (J13 - K13)) / 20</f>
         <v>0.85</v>
       </c>
       <c r="M13">
         <v>3.5</v>
       </c>
       <c r="N13" s="2">
-        <f t="shared" si="2"/>
+        <f>(G13+F13)*L13*(M13+D13+E13+I13+C13)</f>
         <v>51</v>
       </c>
     </row>

</xml_diff>